<commit_message>
Damage Percent for HCF at 0.04192%
</commit_message>
<xml_diff>
--- a/Fatigue Data/Waveform Data.xlsx
+++ b/Fatigue Data/Waveform Data.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:L5001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +411,7 @@
         <v>1000</v>
       </c>
       <c r="E3">
-        <v>285442951.93699998</v>
+        <v>359906330.70300001</v>
       </c>
       <c r="H3">
         <v>0.10101010101010099</v>
@@ -432,7 +432,7 @@
         <v>1000000</v>
       </c>
       <c r="E4">
-        <v>158579417.743</v>
+        <v>199947961.502</v>
       </c>
       <c r="H4">
         <v>0.20202020202020199</v>
@@ -442,7 +442,7 @@
       </c>
       <c r="L4">
         <f>(E4-E3)/(D4-D3)</f>
-        <v>-126.99052471871869</v>
+        <v>-160.1184876886887</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -74793,7 +74793,7 @@
         <v>-0.58432262575532701</v>
       </c>
       <c r="H4967">
-        <f>H4966+$H$3</f>
+        <f t="shared" ref="H4967:H5001" si="76">H4966+$H$3</f>
         <v>501.51515151516469</v>
       </c>
       <c r="I4967">
@@ -74808,7 +74808,7 @@
         <v>-0.94976661951671204</v>
       </c>
       <c r="H4968">
-        <f>H4967+$H$3</f>
+        <f t="shared" si="76"/>
         <v>501.61616161617479</v>
       </c>
       <c r="I4968">
@@ -74823,7 +74823,7 @@
         <v>-0.95229170005532104</v>
       </c>
       <c r="H4969">
-        <f>H4968+$H$3</f>
+        <f t="shared" si="76"/>
         <v>501.7171717171849</v>
       </c>
       <c r="I4969">
@@ -74838,7 +74838,7 @@
         <v>-0.59093299930141296</v>
       </c>
       <c r="H4970">
-        <f>H4969+$H$3</f>
+        <f t="shared" si="76"/>
         <v>501.818181818195</v>
       </c>
       <c r="I4970">
@@ -74853,7 +74853,7 @@
         <v>-3.77065638187421E-3</v>
       </c>
       <c r="H4971">
-        <f>H4970+$H$3</f>
+        <f t="shared" si="76"/>
         <v>501.9191919192051</v>
       </c>
       <c r="I4971">
@@ -74868,7 +74868,7 @@
         <v>0.58483250630130701</v>
       </c>
       <c r="H4972">
-        <f>H4971+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.02020202021521</v>
       </c>
       <c r="I4972">
@@ -74883,7 +74883,7 @@
         <v>0.94996310925976901</v>
       </c>
       <c r="H4973">
-        <f>H4972+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.12121212122531</v>
       </c>
       <c r="I4973">
@@ -74898,7 +74898,7 @@
         <v>0.95209971755711897</v>
       </c>
       <c r="H4974">
-        <f>H4973+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.22222222223542</v>
       </c>
       <c r="I4974">
@@ -74913,7 +74913,7 @@
         <v>0.59042590371983295</v>
       </c>
       <c r="H4975">
-        <f>H4974+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.32323232324552</v>
       </c>
       <c r="I4975">
@@ -74928,7 +74928,7 @@
         <v>3.1422159266195301E-3</v>
       </c>
       <c r="H4976">
-        <f>H4975+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.42424242425562</v>
       </c>
       <c r="I4976">
@@ -74943,7 +74943,7 @@
         <v>-0.58534215587192495</v>
       </c>
       <c r="H4977">
-        <f>H4976+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.52525252526573</v>
       </c>
       <c r="I4977">
@@ -74958,7 +74958,7 @@
         <v>-0.95015922382252005</v>
       </c>
       <c r="H4978">
-        <f>H4977+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.62626262627583</v>
       </c>
       <c r="I4978">
@@ -74973,7 +74973,7 @@
         <v>-0.95190735903449297</v>
       </c>
       <c r="H4979">
-        <f>H4978+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.72727272728594</v>
       </c>
       <c r="I4979">
@@ -74988,7 +74988,7 @@
         <v>-0.58991857495419298</v>
       </c>
       <c r="H4980">
-        <f>H4979+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.82828282829604</v>
       </c>
       <c r="I4980">
@@ -75003,7 +75003,7 @@
         <v>-2.5137742303714202E-3</v>
       </c>
       <c r="H4981">
-        <f>H4980+$H$3</f>
+        <f t="shared" si="76"/>
         <v>502.92929292930614</v>
       </c>
       <c r="I4981">
@@ -75018,7 +75018,7 @@
         <v>0.58585157426663703</v>
       </c>
       <c r="H4982">
-        <f>H4981+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.03030303031625</v>
       </c>
       <c r="I4982">
@@ -75033,7 +75033,7 @@
         <v>0.950354963127226</v>
       </c>
       <c r="H4983">
-        <f>H4982+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.13131313132635</v>
       </c>
       <c r="I4983">
@@ -75048,7 +75048,7 @@
         <v>0.95171462456355205</v>
       </c>
       <c r="H4984">
-        <f>H4983+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.23232323233646</v>
       </c>
       <c r="I4984">
@@ -75063,7 +75063,7 @@
         <v>0.58941101320522504</v>
       </c>
       <c r="H4985">
-        <f>H4984+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.33333333334656</v>
       </c>
       <c r="I4985">
@@ -75078,7 +75078,7 @@
         <v>1.8853315413279799E-3</v>
       </c>
       <c r="H4986">
-        <f>H4985+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.43434343435666</v>
       </c>
       <c r="I4986">
@@ -75093,7 +75093,7 @@
         <v>-0.58636076128388503</v>
       </c>
       <c r="H4987">
-        <f>H4986+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.53535353536677</v>
       </c>
       <c r="I4987">
@@ -75108,7 +75108,7 @@
         <v>-0.95055032709644205</v>
       </c>
       <c r="H4988">
-        <f>H4987+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.63636363637687</v>
       </c>
       <c r="I4988">
@@ -75123,7 +75123,7 @@
         <v>-0.95152151422041598</v>
       </c>
       <c r="H4989">
-        <f>H4988+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.73737373738697</v>
       </c>
       <c r="I4989">
@@ -75138,7 +75138,7 @@
         <v>-0.58890321867265205</v>
       </c>
       <c r="H4990">
-        <f>H4989+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.83838383839708</v>
       </c>
       <c r="I4990">
@@ -75153,7 +75153,7 @@
         <v>-1.2568881081424399E-3</v>
       </c>
       <c r="H4991">
-        <f>H4990+$H$3</f>
+        <f t="shared" si="76"/>
         <v>503.93939393940718</v>
       </c>
       <c r="I4991">
@@ -75168,7 +75168,7 @@
         <v>0.58686971672256705</v>
       </c>
       <c r="H4992">
-        <f>H4991+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.04040404041729</v>
       </c>
       <c r="I4992">
@@ -75183,7 +75183,7 @@
         <v>0.950745315653717</v>
       </c>
       <c r="H4993">
-        <f>H4992+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.14141414142739</v>
       </c>
       <c r="I4993">
@@ -75198,7 +75198,7 @@
         <v>0.95132802808135297</v>
       </c>
       <c r="H4994">
-        <f>H4993+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.24242424243749</v>
       </c>
       <c r="I4994">
@@ -75213,7 +75213,7 @@
         <v>0.58839519155702302</v>
       </c>
       <c r="H4995">
-        <f>H4994+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.3434343434476</v>
       </c>
       <c r="I4995">
@@ -75228,7 +75228,7 @@
         <v>6.28444178104094E-4</v>
       </c>
       <c r="H4996">
-        <f>H4995+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.4444444444577</v>
       </c>
       <c r="I4996">
@@ -75243,7 +75243,7 @@
         <v>-0.58737844038167797</v>
       </c>
       <c r="H4997">
-        <f>H4996+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.54545454546781</v>
       </c>
       <c r="I4997">
@@ -75258,7 +75258,7 @@
         <v>-0.95093992872147604</v>
       </c>
       <c r="H4998">
-        <f>H4997+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.64646464647791</v>
       </c>
       <c r="I4998">
@@ -75273,7 +75273,7 @@
         <v>-0.95113416622291702</v>
       </c>
       <c r="H4999">
-        <f>H4998+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.74747474748801</v>
       </c>
       <c r="I4999">
@@ -75288,7 +75288,7 @@
         <v>-0.58788693205971498</v>
       </c>
       <c r="H5000">
-        <f>H4999+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.84848484849812</v>
       </c>
       <c r="I5000">
@@ -75303,7 +75303,7 @@
         <v>1.3333070495890099E-13</v>
       </c>
       <c r="H5001">
-        <f>H5000+$H$3</f>
+        <f t="shared" si="76"/>
         <v>504.94949494950822</v>
       </c>
       <c r="I5001">

</xml_diff>

<commit_message>
Set up SLDWRKs with LCF and HCF
Should run without having to mess with settings.  Just need to modifiy
design to be stronger.
</commit_message>
<xml_diff>
--- a/Fatigue Data/Waveform Data.xlsx
+++ b/Fatigue Data/Waveform Data.xlsx
@@ -359,8 +359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4965" workbookViewId="0">
+      <selection activeCell="D4993" sqref="D4993"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +457,8 @@
         <v>1000000000000000</v>
       </c>
       <c r="E5">
-        <v>158579417.743</v>
+        <f>E4</f>
+        <v>199947961.502</v>
       </c>
       <c r="H5">
         <v>0.30303030303030298</v>

</xml_diff>